<commit_message>
data updated on Aug. 04
</commit_message>
<xml_diff>
--- a/chengdu_covid19.xlsx
+++ b/chengdu_covid19.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxlin\Desktop\lzcovid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E78E2FB-5FB3-4E35-BDC4-F34A3B8A3623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45ECB497-75BF-4BB4-9191-CFA7A09C2636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="4662" windowWidth="20676" windowHeight="11652" xr2:uid="{7E3BE049-1206-4BBB-9327-FC1B07B4BBF7}"/>
+    <workbookView xWindow="2490" yWindow="4248" windowWidth="20598" windowHeight="12318" xr2:uid="{7E3BE049-1206-4BBB-9327-FC1B07B4BBF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C02FDC6-E9FC-4AAE-9BBA-7A98D6755692}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -790,6 +790,71 @@
         <v>0</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A18" s="1">
+        <v>44773</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A19" s="1">
+        <v>44774</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A20" s="1">
+        <v>44775</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A21" s="1">
+        <v>44776</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data updated on Aug.09
</commit_message>
<xml_diff>
--- a/chengdu_covid19.xlsx
+++ b/chengdu_covid19.xlsx
@@ -147,10 +147,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -629,6 +629,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="n">
+        <v>44781</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
data updated on Aug.12
</commit_message>
<xml_diff>
--- a/chengdu_covid19.xlsx
+++ b/chengdu_covid19.xlsx
@@ -147,10 +147,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26:D26"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -643,6 +643,48 @@
         <v>0</v>
       </c>
     </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>44782</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>44783</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="n">
+        <v>44784</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
update on Sep. 02, 2022
</commit_message>
<xml_diff>
--- a/chengdu_covid19.xlsx
+++ b/chengdu_covid19.xlsx
@@ -147,10 +147,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -685,6 +685,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="n">
+        <v>44785</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="n">
+        <v>44786</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>